<commit_message>
changes after feb 2025 analysis
</commit_message>
<xml_diff>
--- a/TECHS-16PrePost.xlsx
+++ b/TECHS-16PrePost.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmatinney/Documents/GitHub/techs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{EF3AE95C-1AA3-4E4A-82AB-E12B87EE5363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{9CBE2A00-A8EC-6A49-8B7B-F385956815EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17420" xr2:uid="{BFF4A78D-673F-EC49-8B82-6B5C5937C022}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1199" uniqueCount="1175">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1197" uniqueCount="1175">
   <si>
     <t>name</t>
   </si>
@@ -4055,7 +4055,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -4064,6 +4064,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -4441,7 +4442,7 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86F722C3-7CDC-3E4F-A019-A19B94C34CE4}">
   <dimension ref="A1:ANJ18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="LA1" workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
@@ -38164,10 +38165,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72231F28-36E6-6145-B11D-3BE72695CE9A}">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:K40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -38203,12 +38204,6 @@
       <c r="I1" t="s">
         <v>1172</v>
       </c>
-      <c r="J1" t="s">
-        <v>1168</v>
-      </c>
-      <c r="K1" t="s">
-        <v>1169</v>
-      </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
@@ -38238,12 +38233,8 @@
       <c r="I2">
         <v>6.4011148539999999E-4</v>
       </c>
-      <c r="J2">
-        <v>1.004607556E-3</v>
-      </c>
-      <c r="K2">
-        <v>9.9972756720000003E-4</v>
-      </c>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
@@ -38273,12 +38264,8 @@
       <c r="I3">
         <v>5.9042351449999997E-4</v>
       </c>
-      <c r="J3">
-        <v>9.7412352499999999E-4</v>
-      </c>
-      <c r="K3">
-        <v>9.7470789119999998E-4</v>
-      </c>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -38308,12 +38295,8 @@
       <c r="I4">
         <v>5.7618392189999999E-4</v>
       </c>
-      <c r="J4">
-        <v>9.6055462270000004E-4</v>
-      </c>
-      <c r="K4">
-        <v>9.4972069489999999E-4</v>
-      </c>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
@@ -38343,12 +38326,8 @@
       <c r="I5">
         <v>7.0627950659999999E-4</v>
       </c>
-      <c r="J5">
-        <v>1.01925966E-3</v>
-      </c>
-      <c r="K5">
-        <v>1.0114037150000001E-3</v>
-      </c>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
@@ -38378,12 +38357,8 @@
       <c r="I6">
         <v>6.0625563929999997E-4</v>
       </c>
-      <c r="J6">
-        <v>1.0214399820000001E-3</v>
-      </c>
-      <c r="K6">
-        <v>1.0081535909999999E-3</v>
-      </c>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
@@ -38413,12 +38388,8 @@
       <c r="I7">
         <v>5.9128214279999996E-4</v>
       </c>
-      <c r="J7">
-        <v>9.9151849330000007E-4</v>
-      </c>
-      <c r="K7">
-        <v>9.8786167660000002E-4</v>
-      </c>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -38448,12 +38419,8 @@
       <c r="I8">
         <v>5.9202090369999999E-4</v>
       </c>
-      <c r="J8">
-        <v>9.5477356979999995E-4</v>
-      </c>
-      <c r="K8">
-        <v>9.6219861960000004E-4</v>
-      </c>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9">
@@ -38483,12 +38450,8 @@
       <c r="I9">
         <v>5.95865977E-4</v>
       </c>
-      <c r="J9">
-        <v>9.462895376E-4</v>
-      </c>
-      <c r="K9">
-        <v>9.7530812049999999E-4</v>
-      </c>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10">
@@ -38518,12 +38481,7 @@
       <c r="I10">
         <v>6.0664995749999998E-4</v>
       </c>
-      <c r="J10">
-        <v>1.002346285E-3</v>
-      </c>
-      <c r="K10">
-        <v>1.013596661E-3</v>
-      </c>
+      <c r="K10" s="8"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11">
@@ -38553,12 +38511,8 @@
       <c r="I11">
         <v>5.9802298319999996E-4</v>
       </c>
-      <c r="J11">
-        <v>9.8191412879999993E-4</v>
-      </c>
-      <c r="K11">
-        <v>1.004566132E-3</v>
-      </c>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12">
@@ -38588,12 +38542,7 @@
       <c r="I12">
         <v>7.4593928000000001E-4</v>
       </c>
-      <c r="J12">
-        <v>9.3549803779999999E-4</v>
-      </c>
-      <c r="K12">
-        <v>9.9741592060000007E-4</v>
-      </c>
+      <c r="J12" s="8"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -38623,12 +38572,8 @@
       <c r="I13">
         <v>6.0035603259999998E-4</v>
       </c>
-      <c r="J13">
-        <v>9.4127891939999996E-4</v>
-      </c>
-      <c r="K13">
-        <v>9.9258144499999993E-4</v>
-      </c>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14">
@@ -38658,12 +38603,8 @@
       <c r="I14">
         <v>5.8053834020000002E-4</v>
       </c>
-      <c r="J14">
-        <v>9.9938358069999998E-4</v>
-      </c>
-      <c r="K14">
-        <v>9.7166563809999995E-4</v>
-      </c>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15">
@@ -38693,12 +38634,8 @@
       <c r="I15">
         <v>6.7132502330000002E-4</v>
       </c>
-      <c r="J15">
-        <v>9.6760330000000003E-4</v>
-      </c>
-      <c r="K15">
-        <v>9.3711164020000002E-4</v>
-      </c>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16">
@@ -38728,12 +38665,8 @@
       <c r="I16">
         <v>5.9632179980000002E-4</v>
       </c>
-      <c r="J16">
-        <v>9.8409583200000008E-4</v>
-      </c>
-      <c r="K16">
-        <v>9.6253865249999997E-4</v>
-      </c>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17">
@@ -38763,12 +38696,68 @@
       <c r="I17">
         <v>5.8806409620000002E-4</v>
       </c>
-      <c r="J17">
-        <v>9.7164657389999995E-4</v>
-      </c>
-      <c r="K17">
-        <v>9.7244351519999998E-4</v>
-      </c>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D20" s="8"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D21" s="8"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D22" s="8"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D23" s="8"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D24" s="8"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D25" s="8"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D26" s="8"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D27" s="8"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D29" s="8"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D30" s="8"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D31" s="8"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D32" s="8"/>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D33" s="8"/>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D34" s="8"/>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D35" s="8"/>
+    </row>
+    <row r="36" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D36" s="8"/>
+    </row>
+    <row r="37" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D37" s="8"/>
+    </row>
+    <row r="38" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D38" s="8"/>
+    </row>
+    <row r="39" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D39" s="8"/>
+    </row>
+    <row r="40" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D40" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>